<commit_message>
R code for Feb 1 forecast errors
</commit_message>
<xml_diff>
--- a/2023SEIS-Proposals/2023-SEIS-Proposals.xlsx
+++ b/2023SEIS-Proposals/2023-SEIS-Proposals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\2023SEIS-Proposals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B2D3A5-ED11-4200-9EFA-87EA573EA2B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3752E9F0-A77A-4456-98CB-1114E619B693}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6230" activeTab="1" xr2:uid="{F538D32F-F9FA-408E-AB2F-811AEA3D3CB9}"/>
   </bookViews>
@@ -439,6 +439,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -459,15 +468,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -15053,8 +15053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADCCAAB-1B22-4789-8EDA-A0B15F44BB8A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15096,31 +15096,31 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="34" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="39"/>
       <c r="H9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="33"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="35"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="22" t="s">
         <v>0</v>
       </c>
@@ -15347,7 +15347,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="16">
@@ -15360,25 +15360,25 @@
       <c r="F4">
         <v>1040</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="34">
         <f>VLOOKUP(F4,'Mead-Elevation-Storage'!$A$5:$B$676,2)/1000000</f>
         <v>6.977665</v>
       </c>
-      <c r="H4" s="43">
+      <c r="H4" s="36">
         <f>VLOOKUP($F4,MeadEvap!$B$2:$H$673,7)/1000000</f>
         <v>0.37858699999945</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="36">
         <f>VLOOKUP($F4,MeadEvap!$B$2:$H$673,6)/1000000</f>
         <v>0.44053759999935999</v>
       </c>
-      <c r="J4" s="40">
+      <c r="J4" s="33">
         <f>AVERAGE(H4:I4)</f>
         <v>0.40956229999940497</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="16">
@@ -15387,25 +15387,25 @@
       <c r="F5">
         <v>1120</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="34">
         <f>VLOOKUP(F5,'Mead-Elevation-Storage'!$A$5:$B$676,2)/1000000</f>
         <v>13.601435345500001</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="36">
         <f>VLOOKUP($F5,MeadEvap!$B$2:$H$673,7)/1000000</f>
         <v>0.5349370224451</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="36">
         <f>VLOOKUP($F5,MeadEvap!$B$2:$H$673,6)/1000000</f>
         <v>0.62247217157248003</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="33">
         <f>AVERAGE(H5:I5)</f>
         <v>0.57870459700879007</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="16">
@@ -15413,7 +15413,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="32" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="16">
@@ -15421,7 +15421,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="32" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="16">
@@ -15429,7 +15429,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="32" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="16">
@@ -15441,7 +15441,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="32" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="16">
@@ -15501,10 +15501,10 @@
       <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="35" t="s">
         <v>54</v>
       </c>
       <c r="I1" t="s">
@@ -49958,22 +49958,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="37"/>
+      <c r="F1" s="42"/>
       <c r="G1" s="12"/>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">

</xml_diff>